<commit_message>
I believe this is fully functioning version 2. Fixes: forest management inputs, wildfire and managed area outputs, developed_all mortality and dead removal, fire intensity is now fire severity. Added: per managed area diagnostics for use by individual practice simulations; rangeland compost long-term effects last as many years as the repeat period; forest management effects last 35 years. Removed: soil c accumulation adjustment due to forest management (changed in the input parameter file)
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="0" windowWidth="29680" windowHeight="15240" tabRatio="500" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="20160" yWindow="0" windowWidth="29680" windowHeight="15240" tabRatio="500" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="sum_allorgc_2010" sheetId="25" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
   <si>
     <t># total population stats and the mean and stddev of the total population SE values</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t># Wildfire and its affect on carbon pools</t>
-  </si>
-  <si>
-    <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below</t>
-  </si>
-  <si>
-    <t># for veg c uptake, leave the private average the same, use the USFS timberland value for USFS and protected to calculate the fraction below</t>
   </si>
   <si>
     <t># Affects of grassland management on soil C exchange</t>
@@ -238,13 +232,7 @@
     <t># Adapted from ca_carbon_lit.xls, which is a literature survey that has a couple of studies vegetated to ag and urban convsersion</t>
   </si>
   <si>
-    <t># noblank/ NA values allowed</t>
-  </si>
-  <si>
     <t># Units: Fraction - no blank/NA values allowed</t>
-  </si>
-  <si>
-    <t># The soilCaccum_frac is the ratio of the average of two plantation values to the average soil accum rate</t>
   </si>
   <si>
     <t># These are generally net values; assume that root mortality and dead pool transfer are captured by these net rates; Seagrass is best estimate from coastal conservancy</t>
@@ -262,9 +250,6 @@
     <t># Affects of soil conservation on cultivated soil C exchange</t>
   </si>
   <si>
-    <t># ag is actually a soil C sink outside of the Delta</t>
-  </si>
-  <si>
     <t># Delta rates are based on peatland cultivated values and the assumption that these practices have the same absolute affect on soil c exchange as for non-peatland</t>
   </si>
   <si>
@@ -272,6 +257,27 @@
   </si>
   <si>
     <t># no blank/NA values allowed</t>
+  </si>
+  <si>
+    <t># no blank/ NA values allowed</t>
+  </si>
+  <si>
+    <t># the scenario mortality fraction is transferred to "Above_harvested_frac" within CALAND to facilitate this management</t>
+  </si>
+  <si>
+    <t># other management options can be specified in this table for the removed mortality</t>
+  </si>
+  <si>
+    <t># ag is actually a soil C sink; except in the Delta, the write_caland_inputs.r script deals with this</t>
+  </si>
+  <si>
+    <t># The soilCaccum_frac assumes a 35-year annualized benefit</t>
+  </si>
+  <si>
+    <t># for veg c uptake, leave the private average the same, use the USFS timberland value for USFS and protected to calculate the fraction below; assumes 35-year annualized benefit</t>
+  </si>
+  <si>
+    <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below; assumes 35-year annualized benefit</t>
   </si>
 </sst>
 </file>
@@ -327,8 +333,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="869">
+  <cellStyleXfs count="871">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1204,7 +1212,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="869">
+  <cellStyles count="871">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1639,6 +1647,7 @@
     <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2073,6 +2082,7 @@
     <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2422,12 +2432,12 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2437,17 +2447,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3227,22 +3237,22 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3252,22 +3262,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4085,27 +4095,27 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4115,12 +4125,12 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4943,7 +4953,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -4958,7 +4968,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -5594,8 +5604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5629,7 +5639,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -5649,22 +5659,22 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -6020,7 +6030,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6049,27 +6059,27 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6292,32 +6302,32 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -6772,8 +6782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6790,37 +6800,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6904,7 +6914,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -6914,7 +6924,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -7012,12 +7022,12 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -7027,17 +7037,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -7822,12 +7832,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -7842,22 +7852,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -8639,12 +8649,12 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -8659,17 +8669,17 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -9468,12 +9478,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -9488,12 +9498,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -10238,12 +10248,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -10258,12 +10268,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11008,12 +11018,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11028,12 +11038,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11778,12 +11788,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11798,12 +11808,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -12548,12 +12558,12 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -12568,22 +12578,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
New implementation includes climate effects, new fire, new non-regeneration, new woodland restoration; includes: climate scalar file creation and read-in (this adjusts veg and soil c accum), fire area file creation and read-in (some carbon is decayed over time, fire severity is modified by management), non-regen distance threshold argument and corresponding updates to land use/cover change and carbon effects (can convert some of high severity fire to non-forest), updated land use/cover transitions that reflect restoration activities and appropriate carbon transfers, new calculation of man_area for restoration activities to ensure available land and limit this area; bug fixes include: man_area_sum calculations and how they are used later on, some carbon transfer in land use/cover change, xls files are now formatted properly, updates to fire fractions for c fate
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="20160" yWindow="0" windowWidth="29680" windowHeight="15240" tabRatio="500" firstSheet="10" activeTab="12"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
   <si>
     <t># total population stats and the mean and stddev of the total population SE values</t>
   </si>
@@ -151,9 +151,6 @@
     <t># Sum of vegetation biomass carbon density in this workbook by land type and ownership class, 2010</t>
   </si>
   <si>
-    <t># soil, litter (and downed dead) conversion losses are from ca_carbon_lit.xlsx</t>
-  </si>
-  <si>
     <t># Adapted from ca_carbon_lit.xls, which is a literature survey</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t># these values are from ca_carbon_lit.xlsx in the conversion source tab</t>
   </si>
   <si>
-    <t># no blank/NA values allowed</t>
-  </si>
-  <si>
     <t># no blank/ NA values allowed</t>
   </si>
   <si>
@@ -271,13 +265,28 @@
     <t># ag is actually a soil C sink; except in the Delta, the write_caland_inputs.r script deals with this</t>
   </si>
   <si>
-    <t># The soilCaccum_frac assumes a 35-year annualized benefit</t>
+    <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below; assumes 35-year annualized benefit</t>
   </si>
   <si>
-    <t># for veg c uptake, leave the private average the same, use the USFS timberland value for USFS and protected to calculate the fraction below; assumes 35-year annualized benefit</t>
+    <t># assume root decay is capture in onging soil accum rates</t>
   </si>
   <si>
-    <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below; assumes 35-year annualized benefit</t>
+    <t># no NA values allowed</t>
+  </si>
+  <si>
+    <t># assume that that the standing dead, downed dead, and litter are volatilized at the rate of total living biomass loss</t>
+  </si>
+  <si>
+    <t># assume that the non-volatilized portion of living biomass (main and understory) goes to dead material that decomposes rapidly</t>
+  </si>
+  <si>
+    <t># The soilCaccum_frac assumes a 20-year annualized benefit</t>
+  </si>
+  <si>
+    <t># for veg c uptake, leave the private average the same, use the USFS timberland value for USFS and protected to calculate the fraction below; assumes 20-year annualized benefit</t>
+  </si>
+  <si>
+    <t># soil, litter (and downed dead) conversion losses are from ca_carbon_lit.xlsx; the fractions to adjust fire severity are from lydersen 2017 and apply for the 20-year benefit period</t>
   </si>
 </sst>
 </file>
@@ -333,8 +342,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="871">
+  <cellStyleXfs count="881">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1212,7 +1231,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="871">
+  <cellStyles count="881">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1648,6 +1667,11 @@
     <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2083,6 +2107,11 @@
     <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2437,7 +2466,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2447,17 +2476,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3237,22 +3266,22 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3262,12 +3291,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3277,7 +3306,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4095,17 +4124,17 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4115,7 +4144,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4125,12 +4154,12 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4953,7 +4982,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -4968,7 +4997,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -5605,7 +5634,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5639,7 +5668,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -5659,22 +5688,22 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -6064,22 +6093,22 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6307,12 +6336,12 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -6327,7 +6356,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -6800,22 +6829,22 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -6830,7 +6859,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6885,7 +6914,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6914,32 +6943,32 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7027,7 +7056,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -7037,17 +7066,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -7832,12 +7861,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -7852,22 +7881,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -8649,12 +8678,12 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -8669,17 +8698,17 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -9478,12 +9507,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -9498,12 +9527,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -10248,12 +10277,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -10268,12 +10297,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11018,12 +11047,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11038,12 +11067,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11788,12 +11817,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11808,12 +11837,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -12558,12 +12587,12 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -12578,22 +12607,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
Updated the headers to reflect the new cultivated data.
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="0" windowWidth="29680" windowHeight="15240" tabRatio="500" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="15220" yWindow="120" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="sum_allorgc_2010" sheetId="25" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
   <si>
     <t># total population stats and the mean and stddev of the total population SE values</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t># Soil carbon accumulation, by land type</t>
-  </si>
-  <si>
-    <t># savanna/woodland is the understory grass NEE and complements to tree accumulation</t>
   </si>
   <si>
     <t># meadow is wet alpine meadow value, although another study indicates that some behave more like grasslands</t>
@@ -124,22 +121,7 @@
     <t># Affects of grassland management on soil C exchange</t>
   </si>
   <si>
-    <t># The grasslands area  C source, so values &lt;1 here mean reduction in emissions</t>
-  </si>
-  <si>
-    <t># These fractions are the ratios of the amended accululation rates to the regular accumulation rates (for the grassland amendment study ryals 2013, the changes were added to the regular rates); apply these ratios to the other grassland components</t>
-  </si>
-  <si>
-    <t># These fractions are the ratio of the average conservation c accum rate and the conventional rate</t>
-  </si>
-  <si>
-    <t># the conservation practices are cover crop, or reduced tillage, or cover crop with reduced tillage</t>
-  </si>
-  <si>
     <t># The savanna/woodland values are tree (stem and roots) accumulation only, but the soil understory value includes all other components (exept mortality) and the two together are the total net exchange; so don't change the understory, but move some tree accum to dead pools</t>
-  </si>
-  <si>
-    <t># Forest net soil c accum is treated as such, without knowing the source</t>
   </si>
   <si>
     <t>#Developed area vegetation management activities and their affect on carbon pools</t>
@@ -217,15 +199,6 @@
     <t># Units: Mega grams per hectare per year; blank = NA = nodata</t>
   </si>
   <si>
-    <t># Positive values are soil carbon accumulation; Adapted from ca_carbon_lit.xls, which is a literature survey</t>
-  </si>
-  <si>
-    <t># Desert is desert shrub NEE, assumed to go into crust and soil as the shrub biomass is not changing in the studies</t>
-  </si>
-  <si>
-    <t># Delta: Fresh_marsh is avg of 15yr-old and 2yr-old with 95% CI, minus avg losses due to methane emissions; Cultivated is assumed to be on peatland</t>
-  </si>
-  <si>
     <t># Adapted from ca_carbon_lit.xls, which is a literature survey that has a couple of studies vegetated to ag and urban convsersion</t>
   </si>
   <si>
@@ -238,18 +211,6 @@
     <t># remove the dead material and assume it all goes to the atmosphere via decay; this is because only above ground is being tracked</t>
   </si>
   <si>
-    <t># Units: Fraction; no blank/NA values allowed</t>
-  </si>
-  <si>
-    <t># Medium frequency is amendment every 10 years, Low frequency is every 30 years</t>
-  </si>
-  <si>
-    <t># Affects of soil conservation on cultivated soil C exchange</t>
-  </si>
-  <si>
-    <t># Delta rates are based on peatland cultivated values and the assumption that these practices have the same absolute affect on soil c exchange as for non-peatland</t>
-  </si>
-  <si>
     <t># these values are from ca_carbon_lit.xlsx in the conversion source tab</t>
   </si>
   <si>
@@ -260,9 +221,6 @@
   </si>
   <si>
     <t># other management options can be specified in this table for the removed mortality</t>
-  </si>
-  <si>
-    <t># ag is actually a soil C sink; except in the Delta, the write_caland_inputs.r script deals with this</t>
   </si>
   <si>
     <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below; assumes 35-year annualized benefit</t>
@@ -287,6 +245,54 @@
   </si>
   <si>
     <t># soil, litter (and downed dead) conversion losses are from ca_carbon_lit.xlsx; the fractions to adjust fire severity are from lydersen 2017 and apply for the 20-year benefit period</t>
+  </si>
+  <si>
+    <t># The below transfers to atmos and soil need to add to the above_removed_frac; for now assume that this loss to atmosphere is the soil2atmos_frac times the above_removed_frac</t>
+  </si>
+  <si>
+    <t># Units: MgC/ha/y; no NA values allowed</t>
+  </si>
+  <si>
+    <t># Based on calculatuons in cultivated_input_calcs.xlsx, which is a literature survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># ag is a soil C sink; except in the Delta. </t>
+  </si>
+  <si>
+    <t># The non-Delta fluxes are based on tomato-cotton rotation with cover crop and/or reduced tillage in San Joaquin Valley (Mitchell et al., 2015) and maize-tomato with cover crop or cover crop and composted manure in Sacramento Valley (Kong et al., 2005).</t>
+  </si>
+  <si>
+    <t># The non-Delta uncertainty ranges are the SD of the individual treatment means, and represent the uncertainty of statewide average soil C fluxes from conventionally managed systems.</t>
+  </si>
+  <si>
+    <t># Since there are no studies of cover crop, reduced tillage or composting in the Delta region, the benefit (0.40±0.2 Mg C/ha/y) from the non-Delta regions was added to the Delta baseline soil C flux to estimate -2.4±2.56 Mg C/ha/y. The uncertainty range represents the propagated error of the non-Delta benefit and Delta baseline soil C flux.</t>
+  </si>
+  <si>
+    <t># Units: Mega grams C per hectare per year; NA = nodata</t>
+  </si>
+  <si>
+    <t># Positive values are soil carbon accumulation; Adapted from ca_carbon_lit.xlsx, which is a literature survey, expcept for cultivated lands which are based on another lit survey in cultivated_input_calcs.xlsx</t>
+  </si>
+  <si>
+    <t># Forest net soil c accum is treated as such, without knowing the source.Savanna/woodland is the understory grass NEE and complements to tree accumulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Non-delta cultivated represents mean net soil C flux of conventionally managed systems in San Joaquin Valley (8-year tomato-cotton, and 30-year chrono-sequence of alfalfa, wheat, maize, cotton, and sugar beets) (Mitchell et al., 2015; Wu et al., 2008), Sacramento Valley (four 10-year systems in irrigated wheat and fallow, rainfed wheat and fallow, wheat-tomato, and maize-tomato) (Kong et al., 2005), and Imperial Valley (90-year chrono-sequence of alfalfa, wheat, corn, and sugar beets, starting as uncultivated native soil) (Wu et al., 2008). </t>
+  </si>
+  <si>
+    <t># fresh marsh is avg of 15yr-old and 2yr-old with 95% CI, minus avg losses due to methane emissions; restored delta fresh wetland. Desert is desert shrub NEE, assumed to go into crust and soil as the shrub biomass is not changing in the studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Delta cultivated soil C flux is the average of mean soil C flux from two rice systems (1-yr and 2-yr studies) and one corn system (1-year study) in Twitchell Island (Hatala et al., 2012 and Knox et al., 2015). </t>
+  </si>
+  <si>
+    <t># These are means of comparable mean and stddev values as available; with some min and max values for comparison. For cultivated lands, the SD are the SD of the individual treatment means.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Net soil C exchange of managed cultivated lands </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># The non-Delta SD are the SD of the individual treatment means, and represent the uncertainty of statewide average soil C fluxes from sultivated lands under a suite of soil conservation practices. </t>
   </si>
 </sst>
 </file>
@@ -342,8 +348,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="881">
+  <cellStyleXfs count="885">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1231,7 +1241,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="881">
+  <cellStyles count="885">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1672,6 +1682,8 @@
     <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2112,6 +2124,8 @@
     <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2461,32 +2475,32 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3266,22 +3280,22 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3291,22 +3305,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4100,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4124,47 +4138,47 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -4972,32 +4986,32 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -5633,8 +5647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5663,52 +5677,52 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6088,27 +6102,27 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6314,7 +6328,7 @@
   <dimension ref="A1:U57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6331,37 +6345,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>68</v>
+      <c r="A6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6812,7 +6826,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6829,37 +6843,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6933,42 +6947,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7051,32 +7065,32 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -7861,12 +7875,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -7881,22 +7895,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -8678,12 +8692,12 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -8698,17 +8712,17 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -9507,12 +9521,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -9527,12 +9541,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -10277,12 +10291,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -10297,12 +10311,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11047,12 +11061,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11067,12 +11081,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -11817,12 +11831,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -11837,12 +11851,12 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -12587,12 +12601,12 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -12607,22 +12621,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
updated forest and urban forest data; fixed extra mortality and understory growth bugs; generalized the control for lulcc and wildfire; added a raw mortality file; changed name of raw individual sim control file; added a raw control file for the original five sims
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="120" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="1660" yWindow="5940" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="sum_allorgc_2010" sheetId="25" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t># Developed is only above ground tree data</t>
   </si>
   <si>
-    <t># The forest values are net above ground live wood volume changes; assume the foliage, branch (and bark), root, and understory stock changes in proportion to exisiting c ratios; the stddev is acually SE; min and max are just from std dev; from christensen 2016 tab; then distributed regionally based on data from hudiburg et al 2009</t>
-  </si>
-  <si>
     <t># Units: Mega grams per hectare per year; blank = NA = nodata</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t># other management options can be specified in this table for the removed mortality</t>
   </si>
   <si>
-    <t># for mortality, leave the private the same, use the noncorporate rate for USFS and protected to estimate the fraction below; assumes 35-year annualized benefit</t>
-  </si>
-  <si>
     <t># assume root decay is capture in onging soil accum rates</t>
   </si>
   <si>
@@ -241,13 +235,7 @@
     <t># The soilCaccum_frac assumes a 20-year annualized benefit</t>
   </si>
   <si>
-    <t># for veg c uptake, leave the private average the same, use the USFS timberland value for USFS and protected to calculate the fraction below; assumes 20-year annualized benefit</t>
-  </si>
-  <si>
     <t># soil, litter (and downed dead) conversion losses are from ca_carbon_lit.xlsx; the fractions to adjust fire severity are from lydersen 2017 and apply for the 20-year benefit period</t>
-  </si>
-  <si>
-    <t># The below transfers to atmos and soil need to add to the above_removed_frac; for now assume that this loss to atmosphere is the soil2atmos_frac times the above_removed_frac</t>
   </si>
   <si>
     <t># Units: MgC/ha/y; no NA values allowed</t>
@@ -294,12 +282,24 @@
   <si>
     <t xml:space="preserve"># The non-Delta SD are the SD of the individual treatment means, and represent the uncertainty of statewide average soil C fluxes from sultivated lands under a suite of soil conservation practices. </t>
   </si>
+  <si>
+    <t># The forest values are net above ground live wood volume changes; assume the foliage, branch (and bark), root, and understory stock changes in proportion to exisiting c ratios; the stddev is acually SE; min and max are just from std dev; from ab1504_data.xlsx based on data from hudiburg et al 2009</t>
+  </si>
+  <si>
+    <t># VegCuptake_frac: this is region and ownership dependend; assumes a finite benefit period (currently 20 years)</t>
+  </si>
+  <si>
+    <t># DeadCaccum_frac: this is region and ownership dependent; assumes a finite benefit period (currently 20 years)</t>
+  </si>
+  <si>
+    <t># the below transfers to atmos and soil are calculated respectively from: above_harvested_frac*soil2Atmos_frac and  above_harvested_frac*(1-soil2Atmos_frac)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +330,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1235,11 +1240,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="885">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3262,7 +3268,7 @@
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3285,7 +3291,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3310,7 +3316,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4114,7 +4120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
@@ -4138,42 +4144,42 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4996,7 +5002,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -5011,7 +5017,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -5647,8 +5653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5682,7 +5688,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -5702,27 +5708,27 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" t="s">
-        <v>70</v>
+      <c r="A10" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6107,22 +6113,22 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6350,32 +6356,32 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6843,37 +6849,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6957,27 +6963,27 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:11">

</xml_diff>

<commit_message>
new nwl input files; some small bug fixes in write_caland_inputs.r and CALAND.r
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="5940" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="12" activeTab="12"/>
+    <workbookView xWindow="21440" yWindow="4400" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="sum_allorgc_2010" sheetId="25" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="87">
   <si>
     <t># total population stats and the mean and stddev of the total population SE values</t>
   </si>
@@ -294,6 +294,9 @@
   <si>
     <t># the below transfers to atmos and soil are calculated respectively from: above_harvested_frac*soil2Atmos_frac and  above_harvested_frac*(1-soil2Atmos_frac)</t>
   </si>
+  <si>
+    <t># above harvested and stand dead harvested and understory and downdead and litter to slash conv fracs need to be 1, and understory to downdead needs to be 0</t>
+  </si>
 </sst>
 </file>
 
@@ -353,8 +356,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="885">
+  <cellStyleXfs count="891">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1247,7 +1256,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="885">
+  <cellStyles count="891">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1690,6 +1699,9 @@
     <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2132,6 +2144,9 @@
     <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4970,7 +4985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5017,12 +5032,12 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -5653,7 +5668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now with developed_all roots
</commit_message>
<xml_diff>
--- a/raw_data/parameter_headers.xlsx
+++ b/raw_data/parameter_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21440" yWindow="4400" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="55000" yWindow="4140" windowWidth="22560" windowHeight="20400" tabRatio="500" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="sum_allorgc_2010" sheetId="25" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t># Vegetation carbon net annual uptake, sans mortality, by land type</t>
   </si>
   <si>
-    <t># Developed is only above ground tree data</t>
-  </si>
-  <si>
     <t># Units: Mega grams per hectare per year; blank = NA = nodata</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t># above harvested and stand dead harvested and understory and downdead and litter to slash conv fracs need to be 1, and understory to downdead needs to be 0</t>
+  </si>
+  <si>
+    <t># Developed values are for total of above and below ground tree biomass</t>
   </si>
 </sst>
 </file>
@@ -3282,8 +3282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3331,7 +3331,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3341,7 +3341,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4159,42 +4159,42 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4985,7 +4985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -5032,12 +5032,12 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -5703,7 +5703,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -5723,27 +5723,27 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6128,22 +6128,22 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6371,32 +6371,32 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6864,37 +6864,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6978,27 +6978,27 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11">

</xml_diff>